<commit_message>
Add My Ads Menu
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -391,10 +391,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,18 +745,18 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>56</v>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -823,7 +823,9 @@
       <c r="B14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
@@ -881,7 +883,9 @@
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="5">
+        <v>10</v>
+      </c>
       <c r="D19" s="5" t="s">
         <v>3</v>
       </c>
@@ -891,7 +895,9 @@
       <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
       <c r="D20" s="5" t="s">
         <v>5</v>
       </c>
@@ -901,7 +907,9 @@
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
       <c r="D21" s="5" t="s">
         <v>5</v>
       </c>
@@ -911,7 +919,9 @@
       <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
       <c r="D22" s="5" t="s">
         <v>5</v>
       </c>
@@ -1013,7 +1023,9 @@
       <c r="B32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C32" s="5"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
       </c>
@@ -1203,7 +1215,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Implement Public Ads Paging
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -824,7 +824,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>5</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>

<commit_message>
Some structure adjustments and update Score protocol
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -670,7 +670,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -932,7 +932,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>5</v>
@@ -956,7 +956,7 @@
         <v>17</v>
       </c>
       <c r="C25" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>5</v>
@@ -992,7 +992,7 @@
         <v>20</v>
       </c>
       <c r="C28" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>5</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>